<commit_message>
Small changes to ftl_items wording - changed Fish to Seafood - and changed the Supply Chain to include changes sent from Zac
</commit_message>
<xml_diff>
--- a/ftl_items.xlsx
+++ b/ftl_items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/GMU DAEN/DAEN 690 - Capstone/Data_Generation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/GMU DAEN/DAEN 690 - Capstone/Data_Generation/GMU-DAEN690-FoodTraceability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{741B496E-95C9-3A48-AC88-508CB756938A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE636D9-E0CB-AC47-BEFC-D5615C7F99A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="860" windowWidth="26840" windowHeight="15940" xr2:uid="{C3B6468C-2512-9046-B643-EC618C2DD1C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="130">
   <si>
     <t>eggs</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Cheese (made from pasteurized milk), fresh soft or soft unripened</t>
-  </si>
-  <si>
     <t>brie</t>
   </si>
   <si>
@@ -167,12 +164,6 @@
     <t>muenster</t>
   </si>
   <si>
-    <t>Cheese (made from pasteurized milk), soft ripened or semi-soft</t>
-  </si>
-  <si>
-    <t>Cheese (made from unpasteurized milk), other than hard cheese[1]</t>
-  </si>
-  <si>
     <t>raw-milk soft cheese</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>mahi mahi</t>
   </si>
   <si>
-    <t>Finfish, histamine-producing species</t>
-  </si>
-  <si>
     <t>grouper</t>
   </si>
   <si>
@@ -317,9 +305,6 @@
     <t>snapper</t>
   </si>
   <si>
-    <t>Finfish, species potentially contaminated with ciguatoxin</t>
-  </si>
-  <si>
     <t>cod</t>
   </si>
   <si>
@@ -338,9 +323,6 @@
     <t>trout</t>
   </si>
   <si>
-    <t>Finfish, species not associated with histamine or ciguatoxin</t>
-  </si>
-  <si>
     <t>shrimp</t>
   </si>
   <si>
@@ -353,9 +335,6 @@
     <t>crayfish</t>
   </si>
   <si>
-    <t>Crustaceans</t>
-  </si>
-  <si>
     <t>oysters</t>
   </si>
   <si>
@@ -365,9 +344,6 @@
     <t>mussels</t>
   </si>
   <si>
-    <t>Molluscan shellfish, bivalves</t>
-  </si>
-  <si>
     <t>egg salad</t>
   </si>
   <si>
@@ -444,6 +420,12 @@
   </si>
   <si>
     <t>Aquaculture</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Seafood</t>
   </si>
 </sst>
 </file>
@@ -815,7 +797,7 @@
   <dimension ref="A1:C1048562"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D291" sqref="D291"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -841,10 +823,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -852,10 +834,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -863,10 +845,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -874,10 +856,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -885,10 +867,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -896,10 +878,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,10 +889,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -918,10 +900,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,10 +911,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -940,10 +922,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -951,10 +933,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -962,10 +944,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,10 +955,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -984,10 +966,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -995,10 +977,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1006,10 +988,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1017,10 +999,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1028,10 +1010,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1039,10 +1021,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1050,10 +1032,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1061,10 +1043,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1072,10 +1054,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1083,10 +1065,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1094,10 +1076,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,10 +1087,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1116,10 +1098,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1127,802 +1109,802 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C63" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C72" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C73" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C74" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C81" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C82" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C83" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C84" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C86" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C87" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C88" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C89" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C91" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C92" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C96" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C98" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C99" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1930,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C101" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1941,10 +1923,10 @@
         <v>0</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C102" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1952,10 +1934,10 @@
         <v>0</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C103" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1963,10 +1945,10 @@
         <v>0</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C104" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -1974,10 +1956,10 @@
         <v>0</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C105" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -1985,10 +1967,10 @@
         <v>0</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C106" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -1996,10 +1978,10 @@
         <v>0</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C107" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2007,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C108" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2018,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C109" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2029,10 +2011,10 @@
         <v>0</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2040,10 +2022,10 @@
         <v>0</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C111" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2051,10 +2033,10 @@
         <v>0</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C112" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2062,10 +2044,10 @@
         <v>0</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C113" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2073,10 +2055,10 @@
         <v>0</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C114" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2084,10 +2066,10 @@
         <v>0</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C115" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2095,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C116" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -2106,10 +2088,10 @@
         <v>1</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C117" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2117,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C118" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2128,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C119" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2139,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C120" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2150,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C121" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -2161,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C122" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -2172,10 +2154,10 @@
         <v>1</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C123" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -2183,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C124" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -2194,10 +2176,10 @@
         <v>1</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C125" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -2205,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C126" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -2216,10 +2198,10 @@
         <v>1</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C127" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -2227,10 +2209,10 @@
         <v>1</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C128" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -2238,10 +2220,10 @@
         <v>1</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C129" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -2249,10 +2231,10 @@
         <v>1</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C130" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -2260,219 +2242,219 @@
         <v>1</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C132" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C133" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C134" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C135" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C136" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C137" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C138" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C139" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C140" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C141" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C142" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C143" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C144" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C145" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C146" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C147" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C148" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C149" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C150" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -2480,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C151" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2491,10 +2473,10 @@
         <v>3</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C152" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -2502,10 +2484,10 @@
         <v>4</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C153" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,10 +2495,10 @@
         <v>2</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C154" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,10 +2506,10 @@
         <v>3</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C155" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2535,10 +2517,10 @@
         <v>4</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C156" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -2546,10 +2528,10 @@
         <v>2</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C157" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -2557,10 +2539,10 @@
         <v>3</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C158" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -2568,10 +2550,10 @@
         <v>4</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C159" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -2579,10 +2561,10 @@
         <v>2</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C160" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -2590,10 +2572,10 @@
         <v>3</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C161" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -2601,1242 +2583,1242 @@
         <v>4</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C162" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C163" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C164" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C165" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C166" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C167" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C168" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C169" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C170" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C171" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C172" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C173" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C174" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C175" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C176" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C177" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C178" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C179" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C180" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>47</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C181" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C182" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C183" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C184" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>56</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C185" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C186" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C187" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C188" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>56</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C189" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C190" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C191" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C192" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>56</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C193" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C194" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C195" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C196" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>61</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C197" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C198" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C199" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C200" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>61</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C201" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C202" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C203" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C204" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>61</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C205" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C206" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C207" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C208" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C209" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C210" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C211" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C212" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C213" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C214" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C215" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C216" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C217" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C218" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C219" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C220" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>76</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="C221" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C222" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C223" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C224" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C225" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C226" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C227" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C228" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C229" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C230" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C231" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C232" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C233" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C234" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C235" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C236" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C237" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C238" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C239" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C240" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C241" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C242" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C243" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C244" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C245" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C246" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C247" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C248" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C249" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C250" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C251" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C252" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C253" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C254" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C255" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C256" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C257" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C258" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C259" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C260" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C261" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C262" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C263" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C264" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C265" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C266" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C267" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C268" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C269" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C270" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C271" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C272" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C273" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="C274" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
@@ -3844,10 +3826,10 @@
         <v>21</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C275" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
@@ -3855,10 +3837,10 @@
         <v>22</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C276" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
@@ -3866,10 +3848,10 @@
         <v>23</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C277" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
@@ -3877,10 +3859,10 @@
         <v>24</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C278" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
@@ -3888,10 +3870,10 @@
         <v>25</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C279" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
@@ -3899,10 +3881,10 @@
         <v>26</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C280" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
@@ -3910,10 +3892,10 @@
         <v>27</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C281" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
@@ -3921,186 +3903,186 @@
         <v>28</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C282" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
+        <v>117</v>
+      </c>
+      <c r="B283" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B283" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C283" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C284" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C285" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C286" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C287" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C288" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C289" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C290" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
+        <v>117</v>
+      </c>
+      <c r="B291" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B291" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C291" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C292" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C293" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C294" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C295" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C296" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C297" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C298" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1048562" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>